<commit_message>
item name/desc string stored in Item, loading item texts better way, new CalculateLevel
</commit_message>
<xml_diff>
--- a/doc/stats.xlsx
+++ b/doc/stats.xlsx
@@ -236,11 +236,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="376409232"/>
-        <c:axId val="376410864"/>
+        <c:axId val="1819091008"/>
+        <c:axId val="1819096448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376409232"/>
+        <c:axId val="1819091008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -282,7 +282,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376410864"/>
+        <c:crossAx val="1819096448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -290,7 +290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376410864"/>
+        <c:axId val="1819096448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,7 +341,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376409232"/>
+        <c:crossAx val="1819091008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2128,165 +2128,190 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>20</v>
       </c>
       <c r="C1">
+        <v>17.5</v>
+      </c>
+      <c r="D1">
         <v>15</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>10</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>5</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="C2">
         <v>20</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4">
         <f>B3+B$1</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:F7" si="0">C3+C$1</f>
+        <f>C3+C$1</f>
+        <v>37.5</v>
+      </c>
+      <c r="D4">
+        <f>D3+D$1</f>
         <v>30</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
+      <c r="E4">
+        <f>E3+E$1</f>
         <v>20</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
+      <c r="F4">
+        <f>F3+F$1</f>
         <v>10</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
+      <c r="G4">
+        <f>G3+G$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B7" si="1">B4+B$1</f>
-        <v>60</v>
+        <f>B4+B$1</f>
+        <v>65</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>C4+C$1</f>
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <f>D4+D$1</f>
         <v>45</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
+      <c r="E5">
+        <f>E4+E$1</f>
         <v>30</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
+      <c r="F5">
+        <f>F4+F$1</f>
         <v>15</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
+      <c r="G5">
+        <f>G4+G$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>B5+B$1</f>
+        <v>85</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>C5+C$1</f>
+        <v>72.5</v>
+      </c>
+      <c r="D6">
+        <f>D5+D$1</f>
         <v>60</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+      <c r="E6">
+        <f>E5+E$1</f>
         <v>40</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="F6">
+        <f>F5+F$1</f>
         <v>20</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
+      <c r="G6">
+        <f>G5+G$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f>B6+B$1</f>
+        <v>105</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>C6+C$1</f>
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <f>D6+D$1</f>
         <v>75</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
+      <c r="E7">
+        <f>E6+E$1</f>
         <v>50</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
+      <c r="F7">
+        <f>F6+F$1</f>
         <v>25</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
+      <c r="G7">
+        <f>G6+G$1</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stat profiles, create character tooltips, new game gui started
</commit_message>
<xml_diff>
--- a/doc/stats.xlsx
+++ b/doc/stats.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
     <sheet name="Arkusz4" sheetId="4" r:id="rId4"/>
+    <sheet name="Arkusz5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>LVL</t>
   </si>
@@ -40,6 +41,60 @@
   </si>
   <si>
     <t>SKILL GAIN</t>
+  </si>
+  <si>
+    <t>CLASS ATTRIBUTES</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>con</t>
+  </si>
+  <si>
+    <t>dex</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>wis</t>
+  </si>
+  <si>
+    <t>cha</t>
+  </si>
+  <si>
+    <t>barbarian</t>
+  </si>
+  <si>
+    <t>bard</t>
+  </si>
+  <si>
+    <t>cleric</t>
+  </si>
+  <si>
+    <t>druid</t>
+  </si>
+  <si>
+    <t>hunter</t>
+  </si>
+  <si>
+    <t>mage</t>
+  </si>
+  <si>
+    <t>monk</t>
+  </si>
+  <si>
+    <t>paladin</t>
+  </si>
+  <si>
+    <t>rogue</t>
+  </si>
+  <si>
+    <t>warrior</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -64,10 +119,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -76,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -100,6 +165,7 @@
   <c:lang val="pl-PL"/>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -218,11 +284,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="59665792"/>
-        <c:axId val="80081280"/>
+        <c:axId val="81423744"/>
+        <c:axId val="83170432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59665792"/>
+        <c:axId val="81423744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -262,14 +328,14 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80081280"/>
+        <c:crossAx val="83170432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80081280"/>
+        <c:axId val="83170432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -318,7 +384,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59665792"/>
+        <c:crossAx val="81423744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -360,7 +426,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -656,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1196,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1275,27 +1341,27 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <f>B4+B$2</f>
+        <f t="shared" ref="B5:G8" si="0">B4+B$2</f>
         <v>45</v>
       </c>
       <c r="C5">
-        <f>C4+C$2</f>
+        <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
       <c r="D5">
-        <f>D4+D$2</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E5">
-        <f>E4+E$2</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F5">
-        <f>F4+F$2</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G5">
-        <f>G4+G$2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1304,27 +1370,27 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <f>B5+B$2</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="C6">
-        <f>C5+C$2</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="D6">
-        <f>D5+D$2</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="E6">
-        <f>E5+E$2</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="F6">
-        <f>F5+F$2</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G6">
-        <f>G5+G$2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1333,27 +1399,27 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <f>B6+B$2</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="C7">
-        <f>C6+C$2</f>
+        <f t="shared" si="0"/>
         <v>72.5</v>
       </c>
       <c r="D7">
-        <f>D6+D$2</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="E7">
-        <f>E6+E$2</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="F7">
-        <f>F6+F$2</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G7">
-        <f>G6+G$2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1362,27 +1428,27 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <f>B7+B$2</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="C8">
-        <f>C7+C$2</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="D8">
-        <f>D7+D$2</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="E8">
-        <f>E7+E$2</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="F8">
-        <f>F7+F$2</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="G8">
-        <f>G7+G$2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1625,4 +1691,341 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+      <c r="C3">
+        <v>70</v>
+      </c>
+      <c r="D3">
+        <v>65</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <f>SUM(B3:G3)</f>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4" s="1">
+        <v>65</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H12" si="0">SUM(B4:G4)</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>70</v>
+      </c>
+      <c r="G5" s="1">
+        <v>55</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>55</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1">
+        <v>40</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>65</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>70</v>
+      </c>
+      <c r="F8">
+        <v>55</v>
+      </c>
+      <c r="G8" s="1">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>55</v>
+      </c>
+      <c r="G9" s="1">
+        <v>45</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>65</v>
+      </c>
+      <c r="D10">
+        <v>45</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>60</v>
+      </c>
+      <c r="G10" s="1">
+        <v>55</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>55</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>70</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1">
+        <v>55</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>55</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12" s="1">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H3:H12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:G12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
debug draw stamina, training, enemies use stamina, updated texts
</commit_message>
<xml_diff>
--- a/doc/stats.xlsx
+++ b/doc/stats.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\carpg\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -12,10 +17,11 @@
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
     <sheet name="Arkusz4" sheetId="4" r:id="rId4"/>
     <sheet name="Arkusz5" sheetId="5" r:id="rId5"/>
+    <sheet name="Arkusz6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>LVL</t>
   </si>
@@ -95,13 +101,46 @@
   </si>
   <si>
     <t>sum</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>base str</t>
+  </si>
+  <si>
+    <t>base end</t>
+  </si>
+  <si>
+    <t>base dex</t>
+  </si>
+  <si>
+    <t>bonus end</t>
+  </si>
+  <si>
+    <t>bonus str</t>
+  </si>
+  <si>
+    <t>bonus dex</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>stamina</t>
+  </si>
+  <si>
+    <t>hp v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,11 +200,21 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -194,10 +243,12 @@
         </a:p>
       </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -282,8 +333,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-545F-40DE-AF03-0BD563489C7C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="81423744"/>
         <c:axId val="83170432"/>
       </c:lineChart>
@@ -292,8 +357,10 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -333,12 +400,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="83170432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -356,6 +425,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -398,6 +468,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -449,7 +520,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -722,23 +799,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -764,7 +841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -778,7 +855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -787,7 +864,7 @@
         <v>4629.637386806462</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -796,7 +873,7 @@
         <v>11856.49166178091</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -805,7 +882,7 @@
         <v>20975.766435393834</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -832,7 +909,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -841,7 +918,7 @@
         <v>43349.408248099462</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -850,7 +927,7 @@
         <v>56149.928708748455</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -859,7 +936,7 @@
         <v>69828.840869167834</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -868,7 +945,7 @@
         <v>84282.549419116724</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -877,7 +954,7 @@
         <v>99429.33695684791</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -886,7 +963,7 @@
         <v>115203.09070228692</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -895,7 +972,7 @@
         <v>131549.2197508743</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -904,7 +981,7 @@
         <v>148421.88303733399</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -913,7 +990,7 @@
         <v>165782.04088478943</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -922,7 +999,7 @@
         <v>183596.04531068858</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -931,7 +1008,7 @@
         <v>201834.59485791443</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -940,7 +1017,7 @@
         <v>220471.94324606165</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -949,7 +1026,7 @@
         <v>239485.28918281701</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -958,7 +1035,7 @@
         <v>258854.29828955818</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -967,7 +1044,7 @@
         <v>278560.72321409581</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -975,7 +1052,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -990,16 +1067,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1010,7 +1087,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1018,7 +1095,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1026,7 +1103,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1034,7 +1111,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1042,7 +1119,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1050,7 +1127,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1058,7 +1135,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1066,7 +1143,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1074,7 +1151,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1085,52 +1162,52 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1141,52 +1218,52 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1197,52 +1274,52 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -1259,21 +1336,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>20</v>
       </c>
@@ -1293,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>25</v>
       </c>
@@ -1313,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1336,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1365,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1394,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -1423,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20</v>
       </c>
@@ -1458,21 +1535,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>8.75</v>
       </c>
@@ -1495,7 +1572,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>25</v>
       </c>
@@ -1518,7 +1595,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1551,7 +1628,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1584,7 +1661,7 @@
         <v>46.25</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -1617,7 +1694,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15</v>
       </c>
@@ -1650,7 +1727,7 @@
         <v>48.75</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1683,7 +1760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -1694,21 +1771,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -1731,7 +1808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1758,7 +1835,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1785,7 +1862,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1812,7 +1889,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1839,7 +1916,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1866,7 +1943,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1893,7 +1970,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1920,7 +1997,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1947,7 +2024,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1974,7 +2051,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2005,9 +2082,9 @@
   <conditionalFormatting sqref="H3:H12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2017,9 +2094,9 @@
   <conditionalFormatting sqref="B3:G12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2028,4 +2105,231 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+      <c r="E1">
+        <v>15</v>
+      </c>
+      <c r="F1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>$B9+$D9*B$1/5</f>
+        <v>65</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:F2" si="0">$B9+$D9*C$1/5</f>
+        <v>71.25</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>83.75</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:F3" si="1">$B10+$D10*B$1/5</f>
+        <v>65</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="1"/>
+        <v>71.25</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>77.5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>83.75</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:F4" si="2">$B11+$D11*B$1/5</f>
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="2"/>
+        <v>58.75</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>62.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>66.25</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <f>500 * (1 + (B14-50)/50)</f>
+        <v>650</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="3">500 * (1 + (C14-50)/50)</f>
+        <v>712.5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="3"/>
+        <v>775</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>837.5</v>
+      </c>
+      <c r="F6">
+        <f>500 * (1 + (F14-50)/50)</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <f>50+B3*2.5+B4*2</f>
+        <v>322.5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:F7" si="4">50+C3*2.5+C4*2</f>
+        <v>345.625</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="4"/>
+        <v>368.75</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
+        <v>391.875</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <f>B3*0.8 + B2*0.2</f>
+        <v>65</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:F14" si="5">C3*0.8 + C2*0.2</f>
+        <v>71.25</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="5"/>
+        <v>77.5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="5"/>
+        <v>83.75</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PR Stamina - Combat (#121)
* unit stamina, water potion effect

* fixed stamina buff tooltip

* stamina effect on running, restoring, stamina in stats

* new file writer/reader, moved some things from todo to github

* stamina wip

* fixed load state calculations, fixed pickup/drop animation depending on walk speed, stamina restore depends on load state

* debug draw stamina, training, enemies use stamina, updated texts

* stamina done
</commit_message>
<xml_diff>
--- a/doc/stats.xlsx
+++ b/doc/stats.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\carpg\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -12,10 +17,11 @@
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
     <sheet name="Arkusz4" sheetId="4" r:id="rId4"/>
     <sheet name="Arkusz5" sheetId="5" r:id="rId5"/>
+    <sheet name="Arkusz6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>LVL</t>
   </si>
@@ -95,13 +101,46 @@
   </si>
   <si>
     <t>sum</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>base str</t>
+  </si>
+  <si>
+    <t>base end</t>
+  </si>
+  <si>
+    <t>base dex</t>
+  </si>
+  <si>
+    <t>bonus end</t>
+  </si>
+  <si>
+    <t>bonus str</t>
+  </si>
+  <si>
+    <t>bonus dex</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>stamina</t>
+  </si>
+  <si>
+    <t>hp v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,11 +200,21 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -194,10 +243,12 @@
         </a:p>
       </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -282,8 +333,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-545F-40DE-AF03-0BD563489C7C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="81423744"/>
         <c:axId val="83170432"/>
       </c:lineChart>
@@ -292,8 +357,10 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -333,12 +400,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="83170432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -356,6 +425,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -398,6 +468,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -449,7 +520,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -722,23 +799,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -764,7 +841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -778,7 +855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -787,7 +864,7 @@
         <v>4629.637386806462</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -796,7 +873,7 @@
         <v>11856.49166178091</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -805,7 +882,7 @@
         <v>20975.766435393834</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -832,7 +909,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -841,7 +918,7 @@
         <v>43349.408248099462</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -850,7 +927,7 @@
         <v>56149.928708748455</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -859,7 +936,7 @@
         <v>69828.840869167834</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -868,7 +945,7 @@
         <v>84282.549419116724</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -877,7 +954,7 @@
         <v>99429.33695684791</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -886,7 +963,7 @@
         <v>115203.09070228692</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -895,7 +972,7 @@
         <v>131549.2197508743</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -904,7 +981,7 @@
         <v>148421.88303733399</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -913,7 +990,7 @@
         <v>165782.04088478943</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -922,7 +999,7 @@
         <v>183596.04531068858</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -931,7 +1008,7 @@
         <v>201834.59485791443</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -940,7 +1017,7 @@
         <v>220471.94324606165</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -949,7 +1026,7 @@
         <v>239485.28918281701</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -958,7 +1035,7 @@
         <v>258854.29828955818</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -967,7 +1044,7 @@
         <v>278560.72321409581</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -975,7 +1052,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -990,16 +1067,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1010,7 +1087,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1018,7 +1095,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1026,7 +1103,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1034,7 +1111,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1042,7 +1119,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1050,7 +1127,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1058,7 +1135,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1066,7 +1143,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1074,7 +1151,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1085,52 +1162,52 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1141,52 +1218,52 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1197,52 +1274,52 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -1259,21 +1336,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>20</v>
       </c>
@@ -1293,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>25</v>
       </c>
@@ -1313,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1336,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1365,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1394,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -1423,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20</v>
       </c>
@@ -1458,21 +1535,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>8.75</v>
       </c>
@@ -1495,7 +1572,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>25</v>
       </c>
@@ -1518,7 +1595,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1551,7 +1628,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1584,7 +1661,7 @@
         <v>46.25</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -1617,7 +1694,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15</v>
       </c>
@@ -1650,7 +1727,7 @@
         <v>48.75</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1683,7 +1760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -1694,21 +1771,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -1731,7 +1808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1758,7 +1835,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1785,7 +1862,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1812,7 +1889,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1839,7 +1916,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1866,7 +1943,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1893,7 +1970,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1920,7 +1997,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1947,7 +2024,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1974,7 +2051,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2005,9 +2082,9 @@
   <conditionalFormatting sqref="H3:H12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2017,9 +2094,9 @@
   <conditionalFormatting sqref="B3:G12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2028,4 +2105,231 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+      <c r="E1">
+        <v>15</v>
+      </c>
+      <c r="F1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>$B9+$D9*B$1/5</f>
+        <v>65</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:F2" si="0">$B9+$D9*C$1/5</f>
+        <v>71.25</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>83.75</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:F3" si="1">$B10+$D10*B$1/5</f>
+        <v>65</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="1"/>
+        <v>71.25</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>77.5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>83.75</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:F4" si="2">$B11+$D11*B$1/5</f>
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="2"/>
+        <v>58.75</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>62.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>66.25</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <f>500 * (1 + (B14-50)/50)</f>
+        <v>650</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="3">500 * (1 + (C14-50)/50)</f>
+        <v>712.5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="3"/>
+        <v>775</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>837.5</v>
+      </c>
+      <c r="F6">
+        <f>500 * (1 + (F14-50)/50)</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <f>50+B3*2.5+B4*2</f>
+        <v>322.5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:F7" si="4">50+C3*2.5+C4*2</f>
+        <v>345.625</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="4"/>
+        <v>368.75</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
+        <v>391.875</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <f>B3*0.8 + B2*0.2</f>
+        <v>65</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:F14" si="5">C3*0.8 + C2*0.2</f>
+        <v>71.25</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="5"/>
+        <v>77.5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="5"/>
+        <v>83.75</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>